<commit_message>
Fix: Planilha está completa, gerando corretamente, entrando em ATS e os abastecimentos estão indo para a bomba correta.
</commit_message>
<xml_diff>
--- a/public/Molde_Vazio.xlsx
+++ b/public/Molde_Vazio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7308d51325c9b149/Documentos/Leonardo/Cidade Transportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B4990D7-FADF-4E72-BE4F-BEBE9765C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F089465-24FF-4EE9-8709-10D82A5471E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,10 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]h:mm"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,25 +113,13 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF172336"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,18 +130,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -198,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -206,45 +179,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
@@ -529,7 +469,7 @@
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75">
+    <row r="1" spans="1:13" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,291 +510,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="12"/>
+    <row r="2" spans="1:13" ht="15">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:15" ht="15">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:15" ht="15">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" ht="15">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:15" ht="15">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="12"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" ht="15">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="12"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" ht="15">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" ht="15">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="12"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" ht="15">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" ht="15">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:15" ht="15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:15" ht="15"/>
-    <row r="14" spans="1:15" ht="15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:15" ht="15">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:15" ht="15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="12"/>
-    </row>
-    <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="10"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="12"/>
-    </row>
-    <row r="18" spans="1:11" ht="15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" ht="15">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" ht="15"/>
-    <row r="21" spans="1:11" ht="15">
-      <c r="A21" s="10"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" ht="15">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="12"/>
-    </row>
-    <row r="23" spans="1:11" ht="15">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" ht="15">
-      <c r="A24" s="10"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" ht="15"/>
-    <row r="26" spans="1:11" ht="15"/>
-    <row r="27" spans="1:11" ht="15"/>
-    <row r="29" spans="1:11" ht="15"/>
-    <row r="30" spans="1:11" ht="15"/>
-    <row r="31" spans="1:11" ht="15"/>
-    <row r="33" ht="15"/>
+    <row r="3" spans="1:13" ht="15"/>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>